<commit_message>
calculate modularity based on reference solution
</commit_message>
<xml_diff>
--- a/results/results_05.09.2023.xlsx
+++ b/results/results_05.09.2023.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Util\doctorat\PhdProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA75769-6C1E-441B-999C-4BD4EC2D90C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7618B45-B956-4D5E-B853-7A4BEC71BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3816" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="14" r:id="rId1"/>
+    <sheet name="05.09" sheetId="14" r:id="rId1"/>
+    <sheet name="15.09" sheetId="15" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'15.09'!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>Ant</t>
   </si>
@@ -74,6 +78,9 @@
     <t>MST</t>
   </si>
   <si>
+    <t>sd_catalina.csv</t>
+  </si>
+  <si>
     <t>sd_ant.csv</t>
   </si>
   <si>
@@ -138,13 +145,145 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_10_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_20_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_30_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_40_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_50_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_60_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_70_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_80_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_90_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_100_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_10_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_20_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_30_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_40_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_50_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_60_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_70_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_80_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_90_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>catalina_git_strength_100_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>Catalina</t>
+  </si>
+  <si>
+    <t>NA- one single cluster</t>
+  </si>
+  <si>
+    <t>sd_hibernate.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_60_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_70_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_80_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_90_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_100_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_10_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_20_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_30_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_40_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_50_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_10_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_20_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_30_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_40_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_50_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_60_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_70_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_80_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_90_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>hibernate_git_strength_100_sd_ld.csv</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +295,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,11 +327,20 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -199,6 +354,15 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -208,8 +372,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,12 +410,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +695,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAAC9A7-310A-41EB-81EC-A547CFD32649}">
-  <dimension ref="A3:J26"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="A3:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,128 +716,136 @@
     <col min="10" max="10" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="1:13" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.224</v>
+      </c>
+      <c r="D6" s="5">
         <v>2.7E-2</v>
       </c>
-      <c r="E6">
-        <v>0.438</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="5">
+        <v>0.433</v>
+      </c>
+      <c r="F6" s="5">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>-0.05</v>
-      </c>
-      <c r="H6">
-        <v>3.4670000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G6" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3.3620000000000001</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.61499999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.85599999999999998</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.16200000000000001</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0.05</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>-0.16</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>2.06</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>2.93</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0.57999999999999996</v>
@@ -677,10 +872,10 @@
         <v>1.5649999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>0.57699999999999996</v>
@@ -707,10 +902,10 @@
         <v>1.3720000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>0.59899999999999998</v>
@@ -737,10 +932,10 @@
         <v>1.222</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>0.61499999999999999</v>
@@ -767,10 +962,10 @@
         <v>1.1879999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0.59399999999999997</v>
@@ -796,11 +991,14 @@
       <c r="J12">
         <v>1.226</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>0.64900000000000002</v>
@@ -827,10 +1025,10 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>0.67500000000000004</v>
@@ -857,10 +1055,10 @@
         <v>1.0740000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>0.61299999999999999</v>
@@ -887,10 +1085,10 @@
         <v>1.1890000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>0.61299999999999999</v>
@@ -920,7 +1118,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>0.316</v>
@@ -937,20 +1135,20 @@
       <c r="G17">
         <v>-0.05</v>
       </c>
-      <c r="H17" t="s">
-        <v>32</v>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I17">
         <v>3.0259999999999998</v>
       </c>
-      <c r="J17" t="s">
-        <v>32</v>
+      <c r="J17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>0.29899999999999999</v>
@@ -967,20 +1165,20 @@
       <c r="G18">
         <v>-0.03</v>
       </c>
-      <c r="H18" t="s">
-        <v>32</v>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I18">
         <v>3.1829999999999998</v>
       </c>
-      <c r="J18" t="s">
-        <v>32</v>
+      <c r="J18" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>0.35299999999999998</v>
@@ -997,20 +1195,20 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" t="s">
-        <v>32</v>
+      <c r="H19" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I19">
         <v>3.077</v>
       </c>
-      <c r="J19" t="s">
-        <v>32</v>
+      <c r="J19" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>0.40300000000000002</v>
@@ -1027,20 +1225,20 @@
       <c r="G20">
         <v>-0.03</v>
       </c>
-      <c r="H20" t="s">
-        <v>32</v>
+      <c r="H20" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I20">
         <v>2.7770000000000001</v>
       </c>
-      <c r="J20" t="s">
-        <v>32</v>
+      <c r="J20" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>0.41099999999999998</v>
@@ -1057,20 +1255,20 @@
       <c r="G21">
         <v>-0.03</v>
       </c>
-      <c r="H21" t="s">
-        <v>32</v>
+      <c r="H21" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I21">
         <v>2.738</v>
       </c>
-      <c r="J21" t="s">
-        <v>32</v>
+      <c r="J21" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>0.29599999999999999</v>
@@ -1087,20 +1285,20 @@
       <c r="G22">
         <v>-0.01</v>
       </c>
-      <c r="H22" t="s">
-        <v>32</v>
+      <c r="H22" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I22">
         <v>3.028</v>
       </c>
-      <c r="J22" t="s">
-        <v>32</v>
+      <c r="J22" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.28000000000000003</v>
@@ -1117,20 +1315,20 @@
       <c r="G23">
         <v>-0.02</v>
       </c>
-      <c r="H23" t="s">
-        <v>32</v>
+      <c r="H23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I23">
         <v>3.0390000000000001</v>
       </c>
-      <c r="J23" t="s">
-        <v>32</v>
+      <c r="J23" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.25600000000000001</v>
@@ -1147,20 +1345,20 @@
       <c r="G24">
         <v>-0.03</v>
       </c>
-      <c r="H24" t="s">
-        <v>32</v>
+      <c r="H24" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I24">
         <v>3.3639999999999999</v>
       </c>
-      <c r="J24" t="s">
-        <v>32</v>
+      <c r="J24" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.25800000000000001</v>
@@ -1177,20 +1375,20 @@
       <c r="G25">
         <v>-0.05</v>
       </c>
-      <c r="H25" t="s">
-        <v>32</v>
+      <c r="H25" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I25">
         <v>3.2519999999999998</v>
       </c>
-      <c r="J25" t="s">
-        <v>32</v>
+      <c r="J25" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>0.25800000000000001</v>
@@ -1207,30 +1405,1453 @@
       <c r="G26">
         <v>-0.05</v>
       </c>
-      <c r="H26" t="s">
-        <v>32</v>
+      <c r="H26" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I26">
         <v>3.2519999999999998</v>
       </c>
-      <c r="J26" t="s">
-        <v>32</v>
+      <c r="J26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>-0.18</v>
+      </c>
+      <c r="H27" s="5">
+        <v>-0.26</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3.07</v>
+      </c>
+      <c r="J27" s="5">
+        <v>3.4049999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="H28" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1.948</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3.2850000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1.958</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.3919999999999999</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1.3919999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1.4279999999999999</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1.4279999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.623</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.623</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="I32" s="3">
+        <v>1.177</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1.177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1.1819999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="J36" s="3">
+        <v>1.3129999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.746</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.746</v>
+      </c>
+      <c r="G37" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.3560000000000001</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.753</v>
+      </c>
+      <c r="F38" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="G38" s="3">
+        <v>-0.06</v>
+      </c>
+      <c r="H38" s="3">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="I38" s="3">
+        <v>2.4359999999999999</v>
+      </c>
+      <c r="J38" s="3">
+        <v>3.9039999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="F39" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G39" s="3">
+        <v>-0.06</v>
+      </c>
+      <c r="H39" s="3">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="I39" s="3">
+        <v>2.496</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="F40" s="3">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G40" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="H40" s="3">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="I40" s="3">
+        <v>2.609</v>
+      </c>
+      <c r="J40" s="3">
+        <v>3.702</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="F41" s="3">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G41" s="3">
+        <v>-0.08</v>
+      </c>
+      <c r="H41" s="3">
+        <v>-0.27</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2.552</v>
+      </c>
+      <c r="J41" s="3">
+        <v>3.6629999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="G42" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="H42" s="3">
+        <v>-0.27</v>
+      </c>
+      <c r="I42" s="3">
+        <v>2.7080000000000002</v>
+      </c>
+      <c r="J42" s="3">
+        <v>3.5750000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="F43" s="3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G43" s="3">
+        <v>-0.13</v>
+      </c>
+      <c r="H43" s="3">
+        <v>-0.26</v>
+      </c>
+      <c r="I43" s="3">
+        <v>2.8530000000000002</v>
+      </c>
+      <c r="J43" s="3">
+        <v>3.4969999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.309</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="F44" s="3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G44" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="H44" s="3">
+        <v>-0.26</v>
+      </c>
+      <c r="I44" s="3">
+        <v>3.0310000000000001</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3.3260000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+      <c r="B45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="F45" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G45" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="H45" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="I45" s="3">
+        <v>2.9660000000000002</v>
+      </c>
+      <c r="J45" s="3">
+        <v>3.4009999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F46" s="3">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G46" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="H46" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="I46" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="J46" s="3">
+        <v>3.238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="F47" s="3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G47" s="3">
+        <v>-0.17</v>
+      </c>
+      <c r="H47" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="I47" s="3">
+        <v>2.9849999999999999</v>
+      </c>
+      <c r="J47" s="3">
+        <v>3.1509999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.314</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G48" s="2">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="H48" s="2">
+        <v>-0.31</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.2130000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="I49" s="3">
+        <v>2.4159999999999999</v>
+      </c>
+      <c r="J49" s="3">
+        <v>3.3290000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.704</v>
+      </c>
+      <c r="J50" s="3">
+        <v>1.9079999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51">
+        <v>0.61</v>
+      </c>
+      <c r="D51">
+        <v>0.61</v>
+      </c>
+      <c r="E51">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F51">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="G51">
+        <v>0.25</v>
+      </c>
+      <c r="H51">
+        <v>0.25</v>
+      </c>
+      <c r="I51">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="J51">
+        <v>1.746</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="D52">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="E52">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="F52">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="G52">
+        <v>0.25</v>
+      </c>
+      <c r="H52">
+        <v>0.25</v>
+      </c>
+      <c r="I52">
+        <v>1.3560000000000001</v>
+      </c>
+      <c r="J52">
+        <v>1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="D53">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="E53">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="F53">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="G53">
+        <v>0.25</v>
+      </c>
+      <c r="H53">
+        <v>0.25</v>
+      </c>
+      <c r="I53">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="J53">
+        <v>1.2310000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0.6</v>
+      </c>
+      <c r="D54">
+        <v>0.6</v>
+      </c>
+      <c r="E54">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="F54">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="G54">
+        <v>0.2</v>
+      </c>
+      <c r="H54">
+        <v>0.2</v>
+      </c>
+      <c r="I54">
+        <v>1.2270000000000001</v>
+      </c>
+      <c r="J54">
+        <v>1.2270000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="D55">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E55">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F55">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="G55">
+        <v>0.19</v>
+      </c>
+      <c r="H55">
+        <v>0.19</v>
+      </c>
+      <c r="I55">
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="J55">
+        <v>1.2350000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="D56">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="E56">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="F56">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="G56">
+        <v>0.18</v>
+      </c>
+      <c r="H56">
+        <v>0.18</v>
+      </c>
+      <c r="I56">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="J56">
+        <v>1.2330000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="D57">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="E57">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="F57">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="G57">
+        <v>0.18</v>
+      </c>
+      <c r="H57">
+        <v>0.18</v>
+      </c>
+      <c r="I57">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="J57">
+        <v>1.2330000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="D58">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="E58">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="F58">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="G58">
+        <v>0.18</v>
+      </c>
+      <c r="H58">
+        <v>0.18</v>
+      </c>
+      <c r="I58">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="J58">
+        <v>1.2330000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="D59">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E59">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H59">
+        <v>-0.32</v>
+      </c>
+      <c r="I59">
+        <v>4.4889999999999999</v>
+      </c>
+      <c r="J59">
+        <v>4.6420000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60">
+        <v>0.32</v>
+      </c>
+      <c r="D60">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E60">
+        <v>0.64</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>-0.27</v>
+      </c>
+      <c r="H60">
+        <v>-0.31</v>
+      </c>
+      <c r="I60">
+        <v>4.0979999999999999</v>
+      </c>
+      <c r="J60">
+        <v>4.4829999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D61">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E61">
+        <v>0.629</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>-0.27</v>
+      </c>
+      <c r="H61">
+        <v>-0.31</v>
+      </c>
+      <c r="I61">
+        <v>3.96</v>
+      </c>
+      <c r="J61">
+        <v>4.4109999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="D62">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E62">
+        <v>0.627</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>-0.27</v>
+      </c>
+      <c r="H62">
+        <v>-0.31</v>
+      </c>
+      <c r="I62">
+        <v>3.9529999999999998</v>
+      </c>
+      <c r="J62">
+        <v>4.3719999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="D63">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E63">
+        <v>0.62</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H63">
+        <v>-0.31</v>
+      </c>
+      <c r="I63">
+        <v>4.2539999999999996</v>
+      </c>
+      <c r="J63">
+        <v>4.3609999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64">
+        <v>0.223</v>
+      </c>
+      <c r="D64">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E64">
+        <v>0.61</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H64">
+        <v>-0.31</v>
+      </c>
+      <c r="I64">
+        <v>4.617</v>
+      </c>
+      <c r="J64">
+        <v>4.3209999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65">
+        <v>0.218</v>
+      </c>
+      <c r="D65">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E65">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H65">
+        <v>-0.31</v>
+      </c>
+      <c r="I65">
+        <v>4.7290000000000001</v>
+      </c>
+      <c r="J65">
+        <v>4.319</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D66">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E66">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H66">
+        <v>-0.31</v>
+      </c>
+      <c r="I66">
+        <v>4.6970000000000001</v>
+      </c>
+      <c r="J66">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D67">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E67">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H67">
+        <v>-0.31</v>
+      </c>
+      <c r="I67">
+        <v>4.6970000000000001</v>
+      </c>
+      <c r="J67">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D68">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E68">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H68">
+        <v>-0.31</v>
+      </c>
+      <c r="I68">
+        <v>4.6970000000000001</v>
+      </c>
+      <c r="J68">
+        <v>4.32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A6:A26"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
+  <mergeCells count="10">
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A6:A26"/>
+    <mergeCell ref="A27:A47"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EA020F-50A3-4512-9210-C765B79DF43D}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.436</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="F4" s="15">
+        <v>-0.04</v>
+      </c>
+      <c r="G4" s="16">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="H4" s="15">
+        <v>3.806</v>
+      </c>
+      <c r="I4" s="16">
+        <v>2.931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F5" s="15">
+        <v>-0.17</v>
+      </c>
+      <c r="G5" s="15">
+        <v>-0.15</v>
+      </c>
+      <c r="H5" s="15">
+        <v>2.9220000000000002</v>
+      </c>
+      <c r="I5" s="15">
+        <v>3.5409999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.161</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F6" s="17">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="G6" s="17">
+        <v>-0.22</v>
+      </c>
+      <c r="H6" s="17">
+        <v>4.6829999999999998</v>
+      </c>
+      <c r="I6" s="17">
+        <v>4.2830000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>